<commit_message>
updated the references with index formula.
</commit_message>
<xml_diff>
--- a/Fulcrum_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-Correspondence.xlsx
+++ b/Fulcrum_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-Correspondence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FUL_PREPROD_DEC8\Fulcrum_PreProd_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS_GIT_FUL\Fulcrum_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -292,24 +292,73 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Username</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Account Name</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>spinstall</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>spinstall</v>
+          </cell>
+        </row>
         <row r="3">
+          <cell r="B3" t="str">
+            <v>qaleapthought@gmail.com</v>
+          </cell>
           <cell r="D3" t="str">
             <v>John Young g.com</v>
           </cell>
         </row>
         <row r="4">
+          <cell r="B4" t="str">
+            <v>qaleapthought@yahoo.com</v>
+          </cell>
           <cell r="D4" t="str">
             <v>John Kenndy Y.Com</v>
           </cell>
         </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>leaptestsubsite@gmail.com</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>QASubsiteUser Gmail</v>
+          </cell>
+        </row>
         <row r="6">
+          <cell r="B6" t="str">
+            <v>leaptestsubsite@yahoo.com</v>
+          </cell>
           <cell r="D6" t="str">
             <v>QASubsiteUser YahooCom</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>@@</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>@@</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
             <v>QASubsiteUser Gmail@@John Kenndy Y.Com</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>shaikk@leapthought.co.nz</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Shaik Ahamed</v>
           </cell>
         </row>
       </sheetData>
@@ -321,6 +370,11 @@
         </row>
       </sheetData>
       <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Doc Name</v>
+          </cell>
+        </row>
         <row r="2">
           <cell r="B2" t="str">
             <v>Design</v>
@@ -336,6 +390,11 @@
             <v>WNC-INF1-JTC-AR-CVI-001995.docx@@WNC-INF1-JTC-ATH-DRG-002138.docx</v>
           </cell>
         </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>BrowseDocument.docx</v>
+          </cell>
+        </row>
         <row r="6">
           <cell r="B6" t="str">
             <v>AutomationFolder</v>
@@ -349,6 +408,11 @@
         <row r="8">
           <cell r="B8" t="str">
             <v>WNC-INF1-C1-AR-CER-001617.docx@@WNC-INF1-C1-AR-CER-001618.docx@@WNC-INF1-C1-AR-CER-001619.docx@@WNC-INF1-C1-AR-CER-001620.docx@@WNC-INF1-C1-AR-CER-001621.docx</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>WNC-INF1-C1-AR-CER-001617.docx@@WNC-INF1-C1-AR-CER-001618.docx@@WNC-INF1-C1-AR-CER-001619.docx@@WNC-INF1-C1-AR-CER-001620.docx@@WNC-INF1-C1-AR-CER-001621.docx@@WNC-INF1-C1-AR-CER-001622.docx@@WNC-INF1-C1-AR-CER-001623.docx@@WNC-INF1-C1-AR-CER-001624.docx@@WNC-INF1-C1-AR-CER-001625.docx@@WNC-INF1-C1-AR-CER-001626.docx</v>
           </cell>
         </row>
         <row r="10">
@@ -982,7 +1046,7 @@
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -997,7 +1061,7 @@
     <col min="15" max="15" width="16.28515625" customWidth="1"/>
     <col min="16" max="16" width="21.42578125" customWidth="1"/>
     <col min="17" max="18" width="16.28515625" customWidth="1"/>
-    <col min="19" max="19" width="40.7109375" customWidth="1"/>
+    <col min="19" max="19" width="74.85546875" customWidth="1"/>
     <col min="20" max="22" width="16.28515625" customWidth="1"/>
     <col min="23" max="23" width="36.5703125" customWidth="1"/>
     <col min="24" max="24" width="16.28515625" customWidth="1"/>
@@ -1105,11 +1169,11 @@
         <v>46</v>
       </c>
       <c r="D2" t="str">
-        <f>[1]user_credentials_test!$D$3</f>
+        <f>INDEX([1]user_credentials_test!D:D,3,1)</f>
         <v>John Young g.com</v>
       </c>
       <c r="E2" t="str">
-        <f>[1]user_credentials_test!$B$8</f>
+        <f>INDEX([1]user_credentials_test!B:B,8,1)</f>
         <v>QASubsiteUser Gmail@@John Kenndy Y.Com</v>
       </c>
       <c r="G2" t="s">
@@ -1150,23 +1214,23 @@
         <v>Design</v>
       </c>
       <c r="S2" t="str">
-        <f>[1]DocumentDetails!B7</f>
+        <f>INDEX([1]DocumentDetails!B:B,7,1)</f>
         <v>WNC-INF1-JTC-AR-DRG-001994.docx@@WNC-INF1-JTC-AR-CVI-002137.docx@@WNC-INF1-JTC-AR-DRG-002144.docx@@WNC-INF1-JTC-AR-DRG-002145.docx@@WNC-INF1-JTC-AR-DRG-002142.docx@@WNC-INF1-JTC-AR-DRG-002143.docx@@WNC-INF1-JTC-AR-DRG-002130.docx@@WNC-INF1-JTC-AR-CVI-002131.docx@@WNC-INF1-JTC-AR-CER-002132.docx@@WNC-INF1-JTC-AR-CER-002133.docx</v>
       </c>
       <c r="T2" t="str">
-        <f>[1]DocumentDetails!$B$6</f>
+        <f>INDEX([1]DocumentDetails!B:B,6,1)</f>
         <v>AutomationFolder</v>
       </c>
       <c r="U2" t="str">
-        <f>[1]DocumentDetails!B2</f>
+        <f>INDEX([1]DocumentDetails!B:B,2,1)</f>
         <v>Design</v>
       </c>
       <c r="V2" t="str">
-        <f>[1]DocumentDetails!$B$6</f>
+        <f>INDEX([1]DocumentDetails!B:B,6,1)</f>
         <v>AutomationFolder</v>
       </c>
       <c r="W2" t="str">
-        <f>[1]DocumentDetails!B4</f>
+        <f>INDEX([1]DocumentDetails!B:B,4,1)</f>
         <v>WNC-INF1-JTC-AR-CVI-001995.docx@@WNC-INF1-JTC-ATH-DRG-002138.docx</v>
       </c>
       <c r="Y2" t="s">
@@ -1184,11 +1248,11 @@
         <v>22</v>
       </c>
       <c r="D3" t="str">
-        <f>[1]user_credentials_test!$D$3</f>
+        <f>INDEX([1]user_credentials_test!D:D,3,1)</f>
         <v>John Young g.com</v>
       </c>
       <c r="E3" t="str">
-        <f>[1]user_credentials_test!$D$4</f>
+        <f>INDEX([1]user_credentials_test!D:D,4,1)</f>
         <v>John Kenndy Y.Com</v>
       </c>
       <c r="G3" t="s">
@@ -1230,23 +1294,23 @@
         <v>Design</v>
       </c>
       <c r="S3" t="str">
-        <f>[1]DocumentDetails!B7</f>
+        <f>INDEX([1]DocumentDetails!B:B,7,1)</f>
         <v>WNC-INF1-JTC-AR-DRG-001994.docx@@WNC-INF1-JTC-AR-CVI-002137.docx@@WNC-INF1-JTC-AR-DRG-002144.docx@@WNC-INF1-JTC-AR-DRG-002145.docx@@WNC-INF1-JTC-AR-DRG-002142.docx@@WNC-INF1-JTC-AR-DRG-002143.docx@@WNC-INF1-JTC-AR-DRG-002130.docx@@WNC-INF1-JTC-AR-CVI-002131.docx@@WNC-INF1-JTC-AR-CER-002132.docx@@WNC-INF1-JTC-AR-CER-002133.docx</v>
       </c>
       <c r="T3" t="str">
-        <f>[1]DocumentDetails!$B$6</f>
+        <f>INDEX([1]DocumentDetails!B:B,6,1)</f>
         <v>AutomationFolder</v>
       </c>
       <c r="U3" t="str">
-        <f>[1]DocumentDetails!B2</f>
+        <f>INDEX([1]DocumentDetails!B:B,2,1)</f>
         <v>Design</v>
       </c>
       <c r="V3" t="str">
-        <f>[1]DocumentDetails!$B$6</f>
+        <f>INDEX([1]DocumentDetails!B:B,6,1)</f>
         <v>AutomationFolder</v>
       </c>
       <c r="W3" t="str">
-        <f>[1]DocumentDetails!B4</f>
+        <f>INDEX([1]DocumentDetails!B:B,4,1)</f>
         <v>WNC-INF1-JTC-AR-CVI-001995.docx@@WNC-INF1-JTC-ATH-DRG-002138.docx</v>
       </c>
       <c r="Y3" t="s">
@@ -1264,11 +1328,11 @@
         <v>30</v>
       </c>
       <c r="D4" t="str">
-        <f>[1]user_credentials_test!$D$6</f>
+        <f>INDEX([1]user_credentials_test!D:D,6,1)</f>
         <v>QASubsiteUser YahooCom</v>
       </c>
       <c r="E4" t="str">
-        <f>[1]user_credentials_test!$B$8</f>
+        <f>INDEX([1]user_credentials_test!B:B,8,1)</f>
         <v>QASubsiteUser Gmail@@John Kenndy Y.Com</v>
       </c>
       <c r="G4" t="s">
@@ -1310,23 +1374,23 @@
         <v>File Storage</v>
       </c>
       <c r="S4" t="str">
-        <f>[1]DocumentDetails!$B$8</f>
+        <f>INDEX([1]DocumentDetails!B:B,8,1)</f>
         <v>WNC-INF1-C1-AR-CER-001617.docx@@WNC-INF1-C1-AR-CER-001618.docx@@WNC-INF1-C1-AR-CER-001619.docx@@WNC-INF1-C1-AR-CER-001620.docx@@WNC-INF1-C1-AR-CER-001621.docx</v>
       </c>
       <c r="T4" t="str">
-        <f>[1]DocumentDetails!$B$6</f>
+        <f>INDEX([1]DocumentDetails!B:B,6,1)</f>
         <v>AutomationFolder</v>
       </c>
       <c r="U4" t="str">
-        <f>[1]DocumentDetails!$B$11</f>
+        <f>INDEX([1]DocumentDetails!B:B,11,1)</f>
         <v>File Storage</v>
       </c>
       <c r="V4" t="str">
-        <f>[1]DocumentDetails!$B$6</f>
+        <f>INDEX([1]DocumentDetails!B:B,6,1)</f>
         <v>AutomationFolder</v>
       </c>
       <c r="W4" t="str">
-        <f>[1]DocumentDetails!$B$10</f>
+        <f>INDEX([1]DocumentDetails!B:B,10,1)</f>
         <v>WNC-INF1-C1-AR-CVI-001627.docx@@WNC-INF1-C1-AR-CVI-001628.docx</v>
       </c>
       <c r="Y4" t="s">

</xml_diff>